<commit_message>
Add princess assets for Walk[20] and Idle[16].
</commit_message>
<xml_diff>
--- a/JSON/Levels14MoveList.xlsx
+++ b/JSON/Levels14MoveList.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1090E962-76C3-2846-8D05-4E8108CAAC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571EB881-C6F0-B343-890F-EF08BF884144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csvjson" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18571" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18586" uniqueCount="167">
   <si>
     <t>health</t>
   </si>
@@ -505,11 +505,44 @@
   <si>
     <t>R,L,D,R,R,U,R,U,U,R,R,D,R,R,U,U,U,L,U,L,D,R,U,R,D,R,R,U,U,D</t>
   </si>
+  <si>
+    <t>D,D,R,L,L,U,U,R</t>
+  </si>
+  <si>
+    <t>D,L,L,U,U,D,R,R,U</t>
+  </si>
+  <si>
+    <t>R,U,L,D,L,R,U</t>
+  </si>
+  <si>
+    <t>R,D,U,D,L,R,D,D</t>
+  </si>
+  <si>
+    <t>D,D,R,R,U,D</t>
+  </si>
+  <si>
+    <t>R,D</t>
+  </si>
+  <si>
+    <t>R,D,L</t>
+  </si>
+  <si>
+    <t>D,U,R,D</t>
+  </si>
+  <si>
+    <t>R,R,D,D,L,R,U</t>
+  </si>
+  <si>
+    <t>D,D,R,U,R,D,L,U,L</t>
+  </si>
+  <si>
+    <t>R,L,D,R,D</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1433,14 +1466,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CB486"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="J39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B52" sqref="B52"/>
+      <selection pane="bottomRight" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8897,14 +8930,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B70" s="4"/>
+      <c r="B70" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="C70" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D70" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" s="6">
         <f t="shared" si="11"/>
@@ -9004,14 +9039,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B71" s="4"/>
+      <c r="B71" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="C71" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D71" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="6">
         <f t="shared" si="11"/>
@@ -9111,14 +9148,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B72" s="4"/>
+      <c r="B72" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="C72" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D72" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72" s="6">
         <f t="shared" si="11"/>
@@ -9218,14 +9257,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B73" s="4"/>
+      <c r="B73" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="C73" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D73" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73" s="6">
         <f t="shared" si="11"/>
@@ -9326,12 +9367,14 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B74" s="4"/>
+      <c r="B74" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="C74" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D74" s="5" t="b">
+        <v>6</v>
+      </c>
+      <c r="D74" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -9433,12 +9476,14 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B75" s="4"/>
+      <c r="B75" s="4" t="s">
+        <v>158</v>
+      </c>
       <c r="C75" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D75" s="5" t="b">
+        <v>7</v>
+      </c>
+      <c r="D75" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -9538,12 +9583,14 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B76" s="4"/>
+      <c r="B76" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="C76" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D76" s="5" t="b">
+        <v>8</v>
+      </c>
+      <c r="D76" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -9645,12 +9692,14 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B77" s="4"/>
+      <c r="B77" s="4" t="s">
+        <v>160</v>
+      </c>
       <c r="C77" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D77" s="5" t="b">
+        <v>6</v>
+      </c>
+      <c r="D77" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -9752,14 +9801,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B78" s="4"/>
+      <c r="B78" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="C78" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" s="6">
         <f t="shared" si="11"/>
@@ -9846,14 +9897,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B79" s="4"/>
+      <c r="B79" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="C79" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D79" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" s="6">
         <f t="shared" si="11"/>
@@ -9941,14 +9994,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B80" s="4"/>
+      <c r="B80" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="C80" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D80" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" s="6">
         <f t="shared" si="11"/>
@@ -10038,14 +10093,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B81" s="4"/>
+      <c r="B81" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="C81" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D81" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" s="6">
         <f t="shared" si="11"/>
@@ -10134,14 +10191,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B82" s="4"/>
+      <c r="B82" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="C82" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D82" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82" s="6">
         <f t="shared" si="11"/>
@@ -10234,12 +10293,14 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B83" s="4"/>
+      <c r="B83" s="4" t="s">
+        <v>165</v>
+      </c>
       <c r="C83" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D83" s="5" t="b">
+        <v>9</v>
+      </c>
+      <c r="D83" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -10336,14 +10397,16 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="B84" s="4"/>
+      <c r="B84" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="C84" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D84" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84" s="6">
         <f t="shared" si="11"/>
@@ -79912,7 +79975,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CB486"/>
+  <autoFilter ref="A1:CB486" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Levels14MoveList: Update solutions through 120. ChatEngine: add dispatchWorkItem to closeChat and cancel any scheduled closeChat() calls. It works!! Add fastForward button and feature. Add touch functions. Refactor. PauseResetEngine: remove buttonSpecial and special function (because fast forward now exists on the chat engine.) Change button to gear; remove play/pause sprite. Simplify handleControls - removed callSpecialFunc and goes to openSettingsMenu directly. Refactor. GameScene: remove calls to specialFunction. Add touch functions for chatEngine. Re-enable chat messages.
</commit_message>
<xml_diff>
--- a/JSON/Levels14MoveList.xlsx
+++ b/JSON/Levels14MoveList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0917B812-0A02-3149-9F94-031946474FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4F827A-2A34-7C4D-80FE-6F04D562A783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18605" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18684" uniqueCount="204">
   <si>
     <t>health</t>
   </si>
@@ -588,6 +588,66 @@
   </si>
   <si>
     <t>R,D,L,D,R,R,R</t>
+  </si>
+  <si>
+    <t>D,L,D,R,D,L,L,U,L,R,U,U,D,U,L,L,L,D,R,D,R,D,U,U</t>
+  </si>
+  <si>
+    <t>D,R,R,D,L,U,L,D,R,D,L,R,R,R</t>
+  </si>
+  <si>
+    <t>D,R,D,D,L,R,U,U,U,R,R,D</t>
+  </si>
+  <si>
+    <t>R,L,U,U,D,D,R,R,D,D,U,L</t>
+  </si>
+  <si>
+    <t>R,R,L,L,D,D,R,R,R,D</t>
+  </si>
+  <si>
+    <t>D,U,R,R,R,L,D,D,R,D</t>
+  </si>
+  <si>
+    <t>R,R,R,D,L,D,L,L,D,R,R,R</t>
+  </si>
+  <si>
+    <t>D,R,R,R,U,D,D,L,D,L,L,R,R,U,U,L,U</t>
+  </si>
+  <si>
+    <t>R,U,L,U,D</t>
+  </si>
+  <si>
+    <t>R,R,R,D,L,U,L,D,R</t>
+  </si>
+  <si>
+    <t>D,D,D,R,R,U,L,D,D,L,L</t>
+  </si>
+  <si>
+    <t>D,D,U,D,D,R,U,U,R,L,L,D</t>
+  </si>
+  <si>
+    <t>R,R,D,L,D,L,U,R,D</t>
+  </si>
+  <si>
+    <t>D,U,D,U,R,R,R,L,D,D,D,R</t>
+  </si>
+  <si>
+    <t>R,D,L,D,L,D,R</t>
+  </si>
+  <si>
+    <t>R,D,R,D,L,R,U,L</t>
+  </si>
+  <si>
+    <t>R,R,D,L,R,D,L,R,D</t>
+  </si>
+  <si>
+    <t>R,D,R,D,L,U,D,R</t>
+  </si>
+  <si>
+    <t>R,D,D,U,L,D,D</t>
+  </si>
+  <si>
+    <t>D,R,R,L,R,D,L,R</t>
   </si>
 </sst>
 </file>
@@ -1518,13 +1578,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CB486"/>
+  <dimension ref="A1:CB487"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="J88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B103" sqref="B103"/>
+      <selection pane="bottomRight" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12615,14 +12675,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B104" s="4"/>
+      <c r="B104" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="C104" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D104" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104" s="6">
         <f t="shared" si="11"/>
@@ -12755,14 +12817,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B105" s="4"/>
+      <c r="B105" s="4" t="s">
+        <v>186</v>
+      </c>
       <c r="C105" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D105" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" s="6">
         <f t="shared" si="11"/>
@@ -12895,14 +12959,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B106" s="4"/>
+      <c r="B106" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="C106" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D106" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" s="6">
         <f t="shared" si="11"/>
@@ -13035,14 +13101,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B107" s="4"/>
+      <c r="B107" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="C107" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D107" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" s="6">
         <f t="shared" si="11"/>
@@ -13175,12 +13243,14 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B108" s="4"/>
+      <c r="B108" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="C108" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D108" s="5" t="b">
+        <v>10</v>
+      </c>
+      <c r="D108" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -13305,12 +13375,14 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B109" s="4"/>
+      <c r="B109" s="4" t="s">
+        <v>190</v>
+      </c>
       <c r="C109" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D109" s="5" t="b">
+        <v>12</v>
+      </c>
+      <c r="D109" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -13430,14 +13502,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B110" s="4"/>
+      <c r="B110" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="C110" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D110" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" s="6">
         <f t="shared" si="11"/>
@@ -13567,14 +13641,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B111" s="4"/>
+      <c r="B111" s="4" t="s">
+        <v>192</v>
+      </c>
       <c r="C111" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D111" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" s="6">
         <f t="shared" si="11"/>
@@ -13707,14 +13783,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B112" s="4"/>
+      <c r="B112" s="4" t="s">
+        <v>193</v>
+      </c>
       <c r="C112" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D112" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" s="6">
         <f t="shared" si="11"/>
@@ -13826,12 +13904,14 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B113" s="4"/>
+      <c r="B113" s="4" t="s">
+        <v>194</v>
+      </c>
       <c r="C113" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D113" s="5" t="b">
+        <v>11</v>
+      </c>
+      <c r="D113" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -13948,14 +14028,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B114" s="4"/>
+      <c r="B114" s="4" t="s">
+        <v>195</v>
+      </c>
       <c r="C114" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D114" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E114" s="6">
         <f t="shared" si="11"/>
@@ -14077,12 +14159,14 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B115" s="4"/>
+      <c r="B115" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="C115" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D115" s="5" t="b">
+        <v>9</v>
+      </c>
+      <c r="D115" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -14204,12 +14288,14 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B116" s="4"/>
+      <c r="B116" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="C116" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D116" s="5" t="b">
+        <v>12</v>
+      </c>
+      <c r="D116" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -14332,14 +14418,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B117" s="4"/>
+      <c r="B117" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="C117" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D117" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E117" s="6">
         <f t="shared" si="11"/>
@@ -14449,14 +14537,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B118" s="4"/>
+      <c r="B118" s="4" t="s">
+        <v>199</v>
+      </c>
       <c r="C118" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D118" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118" s="6">
         <f t="shared" si="11"/>
@@ -14572,12 +14662,14 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B119" s="4"/>
+      <c r="B119" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="C119" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D119" s="5" t="b">
+        <v>9</v>
+      </c>
+      <c r="D119" s="10" t="b">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -14691,14 +14783,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B120" s="4"/>
+      <c r="B120" s="4" t="s">
+        <v>201</v>
+      </c>
       <c r="C120" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D120" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120" s="6">
         <f t="shared" si="11"/>
@@ -14812,14 +14906,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B121" s="4"/>
+      <c r="B121" s="4" t="s">
+        <v>202</v>
+      </c>
       <c r="C121" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D121" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121" s="6">
         <f t="shared" si="11"/>
@@ -14937,14 +15033,16 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B122" s="4"/>
+      <c r="B122" s="4" t="s">
+        <v>203</v>
+      </c>
       <c r="C122" s="5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D122" s="5" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E122" s="6">
         <f t="shared" si="11"/>
@@ -72613,7 +72711,7 @@
         <v>0</v>
       </c>
       <c r="E452" s="6">
-        <f t="shared" ref="E452:E486" si="41">E451+1</f>
+        <f t="shared" ref="E452:E487" si="41">E451+1</f>
         <v>450</v>
       </c>
       <c r="F452" s="6">
@@ -80061,6 +80159,221 @@
       </c>
       <c r="CB486" s="9" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="487" spans="1:80" x14ac:dyDescent="0.2">
+      <c r="A487" s="3">
+        <f t="shared" ref="A487" si="43">COUNTA(I487:N487)</f>
+        <v>6</v>
+      </c>
+      <c r="B487" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C487" s="5">
+        <f t="shared" ref="C487" si="44">LEN(B487)-LEN(SUBSTITUTE(B487,",",""))+1</f>
+        <v>24</v>
+      </c>
+      <c r="D487" s="10" t="b">
+        <f t="shared" ref="D487" si="45">C487=G487</f>
+        <v>0</v>
+      </c>
+      <c r="E487" s="6">
+        <f t="shared" si="41"/>
+        <v>485</v>
+      </c>
+      <c r="F487" s="6">
+        <f t="shared" ref="F487" si="46">E487</f>
+        <v>485</v>
+      </c>
+      <c r="G487" s="7">
+        <v>30</v>
+      </c>
+      <c r="H487" s="7">
+        <v>1</v>
+      </c>
+      <c r="I487" t="s">
+        <v>88</v>
+      </c>
+      <c r="J487" t="s">
+        <v>81</v>
+      </c>
+      <c r="K487" t="s">
+        <v>88</v>
+      </c>
+      <c r="L487" t="s">
+        <v>89</v>
+      </c>
+      <c r="M487" t="s">
+        <v>88</v>
+      </c>
+      <c r="N487" t="s">
+        <v>89</v>
+      </c>
+      <c r="O487" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="P487" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q487" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="R487" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="S487" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="T487" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="U487" t="s">
+        <v>81</v>
+      </c>
+      <c r="V487" t="s">
+        <v>88</v>
+      </c>
+      <c r="W487" t="s">
+        <v>88</v>
+      </c>
+      <c r="X487" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y487" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z487" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA487" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB487" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC487" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD487" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE487" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF487" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG487" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH487" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI487" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ487" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK487" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL487" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM487" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN487" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO487" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP487" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AQ487" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR487" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS487" t="s">
+        <v>78</v>
+      </c>
+      <c r="AT487" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU487" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW487" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY487" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AZ487" s="9"/>
+      <c r="BA487" s="9"/>
+      <c r="BB487" s="9"/>
+      <c r="BC487" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD487" s="9"/>
+      <c r="BF487" t="s">
+        <v>78</v>
+      </c>
+      <c r="BG487" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH487" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI487" t="s">
+        <v>80</v>
+      </c>
+      <c r="BJ487" t="s">
+        <v>86</v>
+      </c>
+      <c r="BK487" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="BL487" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="BM487" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="BN487" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="BO487" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="BP487" s="9"/>
+      <c r="BT487" t="s">
+        <v>78</v>
+      </c>
+      <c r="BU487" t="s">
+        <v>83</v>
+      </c>
+      <c r="BV487" t="s">
+        <v>87</v>
+      </c>
+      <c r="BW487" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BX487" s="9"/>
+      <c r="BY487" s="9"/>
+      <c r="BZ487" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="CA487" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="CB487" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Levels14MoveList: Update move for Lv 403. ChatEngine: add x3 multiplier to scale for avatarSprite and fastForwardSprite, and in LevelSkipEngine. PurchasePage: add x3 multiplier to imageScale. SettingsRadioNode: divide by 3 multiplier to radioStatus (why are we dividing here, but multiplying elsewhere by 3?) Assets: add a BUNCH of 2x, 3x images. LaunchScene: add x3 multiplier to moonSprite scale. MoonSprite: remove 9th frame, only 0...8. ParallaxSprite: add x3 multiplier to sprite.scale GameboardSprite: change hintBorder to 512x512 and divide 1/3 in the scale (again, why divide and not multiply???) PlayerSprite: divide by 3 in animationMove in startSwordAnimation, otherwise dragon moves too far.
</commit_message>
<xml_diff>
--- a/JSON/Levels14MoveList.xlsx
+++ b/JSON/Levels14MoveList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4F827A-2A34-7C4D-80FE-6F04D562A783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC41C0D-8536-FA4B-A890-FA68567547DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1581,10 +1581,10 @@
   <dimension ref="A1:CB487"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="J385" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B123" sqref="B123"/>
+      <selection pane="bottomRight" activeCell="G405" sqref="G405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -62304,7 +62304,7 @@
         <v>403</v>
       </c>
       <c r="G405" s="7">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H405" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
GameEngine: Add an animation at the beginning of the level to pulse health if starting health > 1.
</commit_message>
<xml_diff>
--- a/JSON/Levels14MoveList.xlsx
+++ b/JSON/Levels14MoveList.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5F221599-560E-2F4E-992F-A686507F88BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC28C1A-9FA6-0E4C-8E31-1897412B108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57020" yWindow="3240" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="57020" yWindow="3240" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csvjson" sheetId="1" r:id="rId1"/>
@@ -662,7 +662,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1200,7 +1200,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1231,9 +1231,6 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1589,14 +1586,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CB489"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J341" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="J53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B352" sqref="B352"/>
+      <selection pane="bottomRight" activeCell="H353" sqref="H353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -52231,7 +52228,7 @@
         <v>14</v>
       </c>
       <c r="H353" s="11">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I353" t="s">
         <v>75</v>
@@ -80414,7 +80411,7 @@
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
-      <c r="B488" s="15" t="s">
+      <c r="B488" s="4" t="s">
         <v>205</v>
       </c>
       <c r="C488" s="5">
@@ -80874,7 +80871,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CB489"/>
+  <autoFilter ref="A1:CB489" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
PartyResultsLineItemSprite: Update animateAmount() animation to look more like DisplayLivesSprite increment animation, with more dynamic wait duration.
</commit_message>
<xml_diff>
--- a/JSON/Levels14MoveList.xlsx
+++ b/JSON/Levels14MoveList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC28C1A-9FA6-0E4C-8E31-1897412B108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEB5157-9426-6F4C-A341-B61A091931EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57020" yWindow="3240" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="2440" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csvjson" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18820" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18877" uniqueCount="208">
   <si>
     <t>health</t>
   </si>
@@ -657,6 +657,9 @@
   </si>
   <si>
     <t>U,R,L,D,U,R,U,L,D,L,D,R,D</t>
+  </si>
+  <si>
+    <t>L,U,L,D,R,L,D,D,D,R,L,R,L,L,R,D,U,D,D,U,R,L,L,L</t>
   </si>
 </sst>
 </file>
@@ -1587,13 +1590,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CB489"/>
+  <dimension ref="A1:CB490"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="J466" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H353" sqref="H353"/>
+      <selection pane="bottomRight" activeCell="B491" sqref="B491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -72533,16 +72536,16 @@
     </row>
     <row r="451" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A451" s="3">
-        <f t="shared" ref="A451:A489" si="36">COUNTA(I451:N451)</f>
+        <f t="shared" ref="A451:C490" si="36">COUNTA(I451:N451)</f>
         <v>6</v>
       </c>
       <c r="B451" s="4"/>
       <c r="C451" s="5">
-        <f t="shared" ref="C451:C489" si="37">LEN(B451)-LEN(SUBSTITUTE(B451,",",""))+1</f>
+        <f t="shared" ref="C451:C490" si="37">LEN(B451)-LEN(SUBSTITUTE(B451,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="D451" s="5" t="b">
-        <f t="shared" ref="D451:D489" si="38">C451=G451</f>
+        <f t="shared" ref="D451:D490" si="38">C451=G451</f>
         <v>0</v>
       </c>
       <c r="E451" s="6">
@@ -72741,7 +72744,7 @@
         <v>0</v>
       </c>
       <c r="E452" s="6">
-        <f t="shared" ref="E452:E489" si="39">E451+1</f>
+        <f t="shared" ref="E452:E490" si="39">E451+1</f>
         <v>450</v>
       </c>
       <c r="F452" s="6">
@@ -80868,6 +80871,214 @@
       <c r="CA489" s="13"/>
       <c r="CB489" s="13" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="490" spans="1:80" x14ac:dyDescent="0.2">
+      <c r="A490" s="3">
+        <f t="shared" si="36"/>
+        <v>6</v>
+      </c>
+      <c r="B490" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C490" s="5">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="D490" s="5" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="E490" s="6">
+        <f t="shared" si="39"/>
+        <v>488</v>
+      </c>
+      <c r="F490" s="6">
+        <f t="shared" ref="F490" si="41">E490</f>
+        <v>488</v>
+      </c>
+      <c r="G490" s="11">
+        <v>24</v>
+      </c>
+      <c r="H490" s="11">
+        <v>1</v>
+      </c>
+      <c r="I490" t="s">
+        <v>88</v>
+      </c>
+      <c r="J490" t="s">
+        <v>85</v>
+      </c>
+      <c r="K490" t="s">
+        <v>85</v>
+      </c>
+      <c r="L490" t="s">
+        <v>85</v>
+      </c>
+      <c r="M490" t="s">
+        <v>88</v>
+      </c>
+      <c r="N490" t="s">
+        <v>88</v>
+      </c>
+      <c r="O490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="P490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q490" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="R490" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="S490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="T490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="U490" t="s">
+        <v>88</v>
+      </c>
+      <c r="V490" t="s">
+        <v>85</v>
+      </c>
+      <c r="W490" t="s">
+        <v>85</v>
+      </c>
+      <c r="X490" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y490" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z490" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC490" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD490" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE490" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG490" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH490" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI490" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ490" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK490" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL490" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO490" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP490" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ490" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR490" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS490" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW490" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX490" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY490" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ490" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA490" s="13"/>
+      <c r="BB490" s="13"/>
+      <c r="BC490" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="BD490" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE490" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI490" t="s">
+        <v>90</v>
+      </c>
+      <c r="BJ490" t="s">
+        <v>78</v>
+      </c>
+      <c r="BK490" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BL490" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM490" s="13"/>
+      <c r="BN490" s="13"/>
+      <c r="BO490" s="13"/>
+      <c r="BP490" s="13"/>
+      <c r="BQ490" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR490" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT490" t="s">
+        <v>83</v>
+      </c>
+      <c r="BU490" t="s">
+        <v>78</v>
+      </c>
+      <c r="BV490" t="s">
+        <v>90</v>
+      </c>
+      <c r="BW490" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="BX490" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY490" s="13"/>
+      <c r="BZ490" s="13"/>
+      <c r="CA490" s="13"/>
+      <c r="CB490" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add comments. Update 489 in Move List.
</commit_message>
<xml_diff>
--- a/JSON/Levels14MoveList.xlsx
+++ b/JSON/Levels14MoveList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC83192-42AC-8A43-BD90-62AF5F466FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBCF2D6-268B-394B-92A2-D00567F6EA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40540" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1236,7 +1236,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1267,9 +1267,6 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1632,10 +1629,10 @@
   <dimension ref="A1:CC492"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K239" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="AI473" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C256" sqref="C256"/>
+      <selection pane="bottomRight" activeCell="B491" sqref="B491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34753,7 +34750,7 @@
       <c r="B258" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C258" s="16" t="s">
+      <c r="C258" s="15" t="s">
         <v>214</v>
       </c>
       <c r="D258" s="5">
@@ -34933,10 +34930,10 @@
         <f t="shared" ref="A259:A322" si="21">COUNTA(J259:O259)</f>
         <v>5</v>
       </c>
-      <c r="B259" s="15" t="s">
+      <c r="B259" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="C259" s="15" t="s">
+      <c r="C259" s="4" t="s">
         <v>215</v>
       </c>
       <c r="D259" s="5">
@@ -81676,7 +81673,7 @@
         <v>85</v>
       </c>
       <c r="O491" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="P491" s="12" t="s">
         <v>88</v>
@@ -81751,7 +81748,7 @@
         <v>88</v>
       </c>
       <c r="AN491" s="12" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AO491" s="12" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
SettingsRadioNode, SettingsTapArea, SettingsTapButton: comment out deinit print statement. GameScene: make offlinePlaySprite optional(?). to what avail? OfflinePlaySprite: refactor to eliminate any retain cycles, if any.
</commit_message>
<xml_diff>
--- a/JSON/Levels14MoveList.xlsx
+++ b/JSON/Levels14MoveList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBCF2D6-268B-394B-92A2-D00567F6EA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA8702D-16F8-2648-A9A3-424FBD60F5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40540" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csvjson" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19003" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19065" uniqueCount="220">
   <si>
     <t>health</t>
   </si>
@@ -693,6 +693,9 @@
   </si>
   <si>
     <t>An extra hammer in hand is what you're left with in the end.</t>
+  </si>
+  <si>
+    <t>D,L,D,D,D,R,D,R,U,D,D,D,R,D,R,R,R,U,U,U,R,U,R,L,U,L,U,L,R,D,D,D,D,L,D,L,R</t>
   </si>
 </sst>
 </file>
@@ -1626,19 +1629,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC492"/>
+  <dimension ref="A1:CC493"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="AI473" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="K469" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B491" sqref="B491"/>
+      <selection pane="bottomRight" activeCell="D501" sqref="D501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
@@ -73249,7 +73252,7 @@
         <v>0</v>
       </c>
       <c r="F452" s="6">
-        <f t="shared" ref="F452:F492" si="39">F451+1</f>
+        <f t="shared" ref="F452:F493" si="39">F451+1</f>
         <v>450</v>
       </c>
       <c r="G452" s="6">
@@ -81824,7 +81827,7 @@
     </row>
     <row r="492" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A492" s="3">
-        <f t="shared" ref="A492" si="46">COUNTA(J492:O492)</f>
+        <f t="shared" ref="A492:A493" si="46">COUNTA(J492:O492)</f>
         <v>6</v>
       </c>
       <c r="B492" s="4" t="s">
@@ -82047,6 +82050,227 @@
         <v>82</v>
       </c>
       <c r="CC492" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="493" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A493" s="3">
+        <f t="shared" si="46"/>
+        <v>6</v>
+      </c>
+      <c r="B493" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D493" s="5">
+        <f t="shared" ref="D493" si="50">LEN(B493)-LEN(SUBSTITUTE(B493,",",""))+1</f>
+        <v>37</v>
+      </c>
+      <c r="E493" s="14" t="b">
+        <f t="shared" ref="E493" si="51">D493=H493</f>
+        <v>0</v>
+      </c>
+      <c r="F493" s="6">
+        <f t="shared" si="39"/>
+        <v>491</v>
+      </c>
+      <c r="G493" s="6">
+        <f t="shared" ref="G493" si="52">F493</f>
+        <v>491</v>
+      </c>
+      <c r="H493" s="11">
+        <v>40</v>
+      </c>
+      <c r="I493" s="11">
+        <v>1</v>
+      </c>
+      <c r="J493" t="s">
+        <v>88</v>
+      </c>
+      <c r="K493" t="s">
+        <v>76</v>
+      </c>
+      <c r="L493" t="s">
+        <v>89</v>
+      </c>
+      <c r="M493" t="s">
+        <v>88</v>
+      </c>
+      <c r="N493" t="s">
+        <v>88</v>
+      </c>
+      <c r="O493" t="s">
+        <v>88</v>
+      </c>
+      <c r="P493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q493" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="R493" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="S493" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="T493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="U493" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="V493" t="s">
+        <v>81</v>
+      </c>
+      <c r="W493" t="s">
+        <v>76</v>
+      </c>
+      <c r="X493" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y493" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z493" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA493" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE493" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG493" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH493" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI493" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ493" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK493" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL493" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM493" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO493" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR493" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS493" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT493" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU493" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW493" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX493" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY493" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ493" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA493" s="13"/>
+      <c r="BB493" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BC493" s="13"/>
+      <c r="BD493" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE493" s="13"/>
+      <c r="BG493" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI493" t="s">
+        <v>84</v>
+      </c>
+      <c r="BK493" t="s">
+        <v>87</v>
+      </c>
+      <c r="BL493" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BM493" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="BN493" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BO493" s="13"/>
+      <c r="BP493" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BQ493" s="13"/>
+      <c r="BR493" t="s">
+        <v>78</v>
+      </c>
+      <c r="BS493" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT493" t="s">
+        <v>84</v>
+      </c>
+      <c r="BU493" t="s">
+        <v>78</v>
+      </c>
+      <c r="BV493" t="s">
+        <v>83</v>
+      </c>
+      <c r="BW493" t="s">
+        <v>83</v>
+      </c>
+      <c r="BX493" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="BY493" s="13"/>
+      <c r="BZ493" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CA493" s="13"/>
+      <c r="CB493" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="CC493" s="13" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Levels14MovelList.xlsx thru LV493.
</commit_message>
<xml_diff>
--- a/JSON/Levels14MoveList.xlsx
+++ b/JSON/Levels14MoveList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB90291-C106-074D-AFFA-CD7482D18FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616B41D5-734B-8A41-A0E0-0395395CA04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19153" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19210" uniqueCount="236">
   <si>
     <t>health</t>
   </si>
@@ -742,6 +742,9 @@
   <si>
     <t>D,R,U,R,U,U,L,L</t>
   </si>
+  <si>
+    <t>D,L,D,D,R,R,R,U,U,R,U,U,L,D,U,D,L,U,R,R,D,D,R,D,D,R,U,D</t>
+  </si>
 </sst>
 </file>
 
@@ -1290,7 +1293,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1324,9 +1327,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1686,13 +1686,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC494"/>
+  <dimension ref="A1:CC495"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="K457" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E138" sqref="E138"/>
+      <selection pane="bottomRight" activeCell="B495" sqref="B495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16078,7 +16078,7 @@
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="E128" s="17" t="b">
+      <c r="E128" s="16" t="b">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -73341,7 +73341,7 @@
         <v>0</v>
       </c>
       <c r="F452" s="6">
-        <f t="shared" ref="F452:F494" si="39">F451+1</f>
+        <f t="shared" ref="F452:F495" si="39">F451+1</f>
         <v>450</v>
       </c>
       <c r="G452" s="6">
@@ -82155,7 +82155,7 @@
         <v>37</v>
       </c>
       <c r="E493" s="14" t="b">
-        <f t="shared" ref="E493" si="51">D493=H493</f>
+        <f t="shared" ref="E493:E495" si="51">D493=H493</f>
         <v>0</v>
       </c>
       <c r="F493" s="6">
@@ -82375,7 +82375,7 @@
         <f t="shared" ref="D494" si="54">LEN(B494)-LEN(SUBSTITUTE(B494,",",""))+1</f>
         <v>29</v>
       </c>
-      <c r="E494" s="16" t="b">
+      <c r="E494" s="5" t="b">
         <f t="shared" ref="E494" si="55">D494=H494</f>
         <v>1</v>
       </c>
@@ -82605,6 +82605,215 @@
       </c>
       <c r="CC494" s="13" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="495" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A495" s="3">
+        <f t="shared" ref="A495" si="57">COUNTA(J495:O495)</f>
+        <v>6</v>
+      </c>
+      <c r="B495" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D495" s="5">
+        <f t="shared" ref="D495" si="58">LEN(B495)-LEN(SUBSTITUTE(B495,",",""))+1</f>
+        <v>28</v>
+      </c>
+      <c r="E495" s="14" t="b">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="F495" s="6">
+        <f t="shared" si="39"/>
+        <v>493</v>
+      </c>
+      <c r="G495" s="6">
+        <f t="shared" ref="G495" si="59">F495</f>
+        <v>493</v>
+      </c>
+      <c r="H495" s="11">
+        <v>30</v>
+      </c>
+      <c r="I495" s="11">
+        <v>2</v>
+      </c>
+      <c r="J495" t="s">
+        <v>88</v>
+      </c>
+      <c r="K495" t="s">
+        <v>88</v>
+      </c>
+      <c r="L495" t="s">
+        <v>88</v>
+      </c>
+      <c r="M495" t="s">
+        <v>88</v>
+      </c>
+      <c r="N495" t="s">
+        <v>88</v>
+      </c>
+      <c r="O495" t="s">
+        <v>88</v>
+      </c>
+      <c r="P495" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q495" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="R495" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="S495" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="T495" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="U495" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="V495" t="s">
+        <v>88</v>
+      </c>
+      <c r="W495" t="s">
+        <v>85</v>
+      </c>
+      <c r="X495" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y495" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z495" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA495" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB495" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC495" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD495" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE495" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF495" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG495" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH495" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI495" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ495" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK495" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL495" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM495" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN495" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO495" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP495" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ495" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR495" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS495" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT495" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU495" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV495" t="s">
+        <v>83</v>
+      </c>
+      <c r="AX495" t="s">
+        <v>82</v>
+      </c>
+      <c r="AY495" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ495" s="13"/>
+      <c r="BA495" s="13"/>
+      <c r="BB495" s="13"/>
+      <c r="BC495" s="13"/>
+      <c r="BD495" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE495" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="BF495" t="s">
+        <v>83</v>
+      </c>
+      <c r="BJ495" t="s">
+        <v>83</v>
+      </c>
+      <c r="BK495" t="s">
+        <v>82</v>
+      </c>
+      <c r="BL495" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BM495" s="13"/>
+      <c r="BN495" s="13"/>
+      <c r="BO495" s="13"/>
+      <c r="BP495" s="13"/>
+      <c r="BQ495" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BS495" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT495" t="s">
+        <v>83</v>
+      </c>
+      <c r="BV495" t="s">
+        <v>78</v>
+      </c>
+      <c r="BW495" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX495" s="13"/>
+      <c r="BY495" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="BZ495" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="CA495" s="13"/>
+      <c r="CB495" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CC495" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GameViewController: add cusceneIntro. DayTheme: move currentHour to private static property. Add setCurrentHour() function. Refactor. CutsceneIntro: Add this transition from the LaunchScene. LaunchScene: add SpriteXPositions typealias to animateTransition(), and transition*() functions. Work on transitionRunning() function. ParallaxManager: add xOffsetsArray to preserve xOffsets of each layer sprite for a smooth transition to cutsceneIntro(). ParallaxSprite: add SpriteXPositions typealias, used to preserve xOffsets of sprite 0 and sprite 1 as it's scrolling across the screen. pollxOffsets() sets the offsets with where the x position is of both sprites. Files: Update moves lists.
</commit_message>
<xml_diff>
--- a/JSON/Levels14MoveList.xlsx
+++ b/JSON/Levels14MoveList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616B41D5-734B-8A41-A0E0-0395395CA04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44B086C-ACDF-744D-9042-732BD34F2645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45220" yWindow="1060" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csvjson" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19210" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19289" uniqueCount="250">
   <si>
     <t>health</t>
   </si>
@@ -745,6 +745,48 @@
   <si>
     <t>D,L,D,D,R,R,R,U,U,R,U,U,L,D,U,D,L,U,R,R,D,D,R,D,D,R,U,D</t>
   </si>
+  <si>
+    <t>R,R,L,U,L,D,R,U,R,U,D,L,U,L,D,R,D,D,L,U,U,U,D,D</t>
+  </si>
+  <si>
+    <t>R,D,U,R,D,L,U,R</t>
+  </si>
+  <si>
+    <t>D,R,L,U,R,R,R,D</t>
+  </si>
+  <si>
+    <t>R,D,R,D,L,D</t>
+  </si>
+  <si>
+    <t>D,D,R,U,U,L,D,U,L</t>
+  </si>
+  <si>
+    <t>R,D,L,U,R,U,U,D,D,D</t>
+  </si>
+  <si>
+    <t>D,R,R,D,L,L,U,L,D</t>
+  </si>
+  <si>
+    <t>D,R,D,R,U,R,D,D</t>
+  </si>
+  <si>
+    <t>D,D,R,D,L,D,U,U,L</t>
+  </si>
+  <si>
+    <t>D,U,R,D,L,D,R,U,D,R</t>
+  </si>
+  <si>
+    <t>R,R,R,D,L,D,L,D,L,R</t>
+  </si>
+  <si>
+    <t>U,L,D,U,D,U,U,D,D,D,D,R,R,U</t>
+  </si>
+  <si>
+    <t>R,D,D,R,U,D,L</t>
+  </si>
+  <si>
+    <t>R,D,L,U,D,R</t>
+  </si>
 </sst>
 </file>
 
@@ -1293,7 +1335,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1329,6 +1371,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1686,13 +1731,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC495"/>
+  <dimension ref="A1:CC496"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K457" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="K113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B495" sqref="B495"/>
+      <selection pane="bottomRight" activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17485,15 +17530,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B139" s="4"/>
+      <c r="B139" s="4" t="s">
+        <v>237</v>
+      </c>
       <c r="C139" s="4"/>
       <c r="D139" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E139" s="5" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F139" s="6">
         <f t="shared" si="14"/>
@@ -17610,15 +17657,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B140" s="4"/>
+      <c r="B140" s="4" t="s">
+        <v>238</v>
+      </c>
       <c r="C140" s="4"/>
       <c r="D140" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E140" s="5" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F140" s="6">
         <f t="shared" si="14"/>
@@ -17740,15 +17789,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B141" s="4"/>
+      <c r="B141" s="4" t="s">
+        <v>239</v>
+      </c>
       <c r="C141" s="4"/>
       <c r="D141" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E141" s="5" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F141" s="6">
         <f t="shared" si="14"/>
@@ -17867,15 +17918,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B142" s="4"/>
+      <c r="B142" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="C142" s="4"/>
       <c r="D142" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E142" s="5" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F142" s="6">
         <f t="shared" si="14"/>
@@ -17992,15 +18045,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B143" s="4"/>
+      <c r="B143" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="C143" s="4"/>
       <c r="D143" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E143" s="5" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F143" s="6">
         <f t="shared" si="14"/>
@@ -18115,13 +18170,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B144" s="4"/>
+      <c r="B144" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="C144" s="4"/>
       <c r="D144" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E144" s="5" t="b">
+        <v>6</v>
+      </c>
+      <c r="E144" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -18238,13 +18295,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B145" s="4"/>
+      <c r="B145" s="4" t="s">
+        <v>242</v>
+      </c>
       <c r="C145" s="4"/>
       <c r="D145" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E145" s="5" t="b">
+        <v>9</v>
+      </c>
+      <c r="E145" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -18358,13 +18417,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B146" s="4"/>
+      <c r="B146" s="4" t="s">
+        <v>243</v>
+      </c>
       <c r="C146" s="4"/>
       <c r="D146" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E146" s="5" t="b">
+        <v>8</v>
+      </c>
+      <c r="E146" s="16" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -18484,13 +18545,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B147" s="4"/>
+      <c r="B147" s="4" t="s">
+        <v>244</v>
+      </c>
       <c r="C147" s="4"/>
       <c r="D147" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E147" s="5" t="b">
+        <v>9</v>
+      </c>
+      <c r="E147" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -18602,13 +18665,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B148" s="4"/>
+      <c r="B148" s="4" t="s">
+        <v>245</v>
+      </c>
       <c r="C148" s="4"/>
       <c r="D148" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E148" s="5" t="b">
+        <v>10</v>
+      </c>
+      <c r="E148" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -18726,13 +18791,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B149" s="4"/>
+      <c r="B149" s="4" t="s">
+        <v>246</v>
+      </c>
       <c r="C149" s="4"/>
       <c r="D149" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E149" s="5" t="b">
+        <v>10</v>
+      </c>
+      <c r="E149" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -18854,13 +18921,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B150" s="4"/>
+      <c r="B150" s="4" t="s">
+        <v>247</v>
+      </c>
       <c r="C150" s="4"/>
       <c r="D150" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E150" s="5" t="b">
+        <v>14</v>
+      </c>
+      <c r="E150" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -18983,15 +19052,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B151" s="4"/>
+      <c r="B151" s="4" t="s">
+        <v>248</v>
+      </c>
       <c r="C151" s="4"/>
       <c r="D151" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E151" s="5" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F151" s="6">
         <f t="shared" si="14"/>
@@ -19124,15 +19195,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B152" s="4"/>
+      <c r="B152" s="4" t="s">
+        <v>249</v>
+      </c>
       <c r="C152" s="4"/>
       <c r="D152" s="5">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E152" s="5" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F152" s="6">
         <f t="shared" si="14"/>
@@ -73341,7 +73414,7 @@
         <v>0</v>
       </c>
       <c r="F452" s="6">
-        <f t="shared" ref="F452:F495" si="39">F451+1</f>
+        <f t="shared" ref="F452:F496" si="39">F451+1</f>
         <v>450</v>
       </c>
       <c r="G452" s="6">
@@ -82814,6 +82887,235 @@
       </c>
       <c r="CC495" s="13" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="496" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A496" s="3">
+        <f t="shared" ref="A496" si="60">COUNTA(J496:O496)</f>
+        <v>6</v>
+      </c>
+      <c r="B496" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D496" s="5">
+        <f t="shared" ref="D496" si="61">LEN(B496)-LEN(SUBSTITUTE(B496,",",""))+1</f>
+        <v>24</v>
+      </c>
+      <c r="E496" s="17" t="b">
+        <f t="shared" ref="E496" si="62">D496=H496</f>
+        <v>1</v>
+      </c>
+      <c r="F496" s="6">
+        <f t="shared" si="39"/>
+        <v>494</v>
+      </c>
+      <c r="G496" s="6">
+        <f t="shared" ref="G496" si="63">F496</f>
+        <v>494</v>
+      </c>
+      <c r="H496" s="11">
+        <v>24</v>
+      </c>
+      <c r="I496" s="11">
+        <v>1</v>
+      </c>
+      <c r="J496" t="s">
+        <v>88</v>
+      </c>
+      <c r="K496" t="s">
+        <v>88</v>
+      </c>
+      <c r="L496" t="s">
+        <v>88</v>
+      </c>
+      <c r="M496" t="s">
+        <v>88</v>
+      </c>
+      <c r="N496" t="s">
+        <v>88</v>
+      </c>
+      <c r="O496" t="s">
+        <v>88</v>
+      </c>
+      <c r="P496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q496" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="R496" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="S496" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="T496" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="U496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="V496" t="s">
+        <v>88</v>
+      </c>
+      <c r="W496" t="s">
+        <v>85</v>
+      </c>
+      <c r="X496" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y496" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z496" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA496" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC496" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD496" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE496" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF496" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH496" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI496" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ496" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK496" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL496" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM496" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS496" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AT496" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU496" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV496" t="s">
+        <v>83</v>
+      </c>
+      <c r="AW496" t="s">
+        <v>83</v>
+      </c>
+      <c r="AX496" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY496" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ496" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA496" s="13"/>
+      <c r="BB496" s="13"/>
+      <c r="BC496" s="13"/>
+      <c r="BD496" s="13"/>
+      <c r="BE496" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="BF496" t="s">
+        <v>83</v>
+      </c>
+      <c r="BG496" t="s">
+        <v>90</v>
+      </c>
+      <c r="BH496" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI496" t="s">
+        <v>78</v>
+      </c>
+      <c r="BJ496" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK496" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL496" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="BM496" s="13"/>
+      <c r="BN496" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BO496" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BP496" s="13"/>
+      <c r="BQ496" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="BR496" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT496" t="s">
+        <v>87</v>
+      </c>
+      <c r="BV496" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW496" t="s">
+        <v>90</v>
+      </c>
+      <c r="BX496" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="BY496" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BZ496" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="CA496" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="CB496" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CC496" s="13" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>